<commit_message>
update: Iniciação à Programação Linear - trabalho 2
</commit_message>
<xml_diff>
--- a/4-Iniciacao-Programacao-Linear/Aula-01/Avaliacao-2/Exemplo-1.xlsx
+++ b/4-Iniciacao-Programacao-Linear/Aula-01/Avaliacao-2/Exemplo-1.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cintia/Desktop/[UTFPR]/utfpr-emma-repo/4-Iniciacao-Programacao-Linear/Aula-01/Avaliacao-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB55EC33-931B-0544-AE16-34D80B33B7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B69AEBD-9A8D-6441-85A2-F39B3D6F696B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9240" yWindow="500" windowWidth="33000" windowHeight="28660" xr2:uid="{3BE5D73E-422B-5846-AFC5-3512089E8F42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet2!$B$6:$D$7</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$6:$D$7</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet2!$B$13:$D$13</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet2!$B$6:$D$7</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet2!$E$17:$E$18</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$13:$D$13</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$6:$D$7</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$E$17:$E$18</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -32,15 +32,15 @@
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet2!$B$31</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$31</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet2!$B$14:$D$14</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$B$14:$D$14</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet2!$F$17:$F$18</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$F$17:$F$18</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -52,7 +52,7 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -129,7 +129,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -192,29 +192,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -224,17 +224,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -593,9 +589,7 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="15"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
@@ -665,7 +659,7 @@
       <c r="D10" s="6">
         <v>130</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -741,7 +735,7 @@
       <c r="F16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -765,7 +759,7 @@
       <c r="F17" s="8">
         <v>10000</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <f>SUM(F17-E17)</f>
         <v>475</v>
       </c>
@@ -790,7 +784,7 @@
       <c r="F18" s="8">
         <v>5000</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <f>SUM(F18-E18)</f>
         <v>0</v>
       </c>

</xml_diff>